<commit_message>
add pdf and tests
</commit_message>
<xml_diff>
--- a/Planning_prevu-effectif.xlsx
+++ b/Planning_prevu-effectif.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396FD72A-CF13-47F7-A4B8-227D443CF4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BE822D-8313-451F-9A06-EA15DB956A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <definedName name="fin_tâche" localSheetId="0">PlanningProjet!$F1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">PlanningProjet!$4:$6</definedName>
     <definedName name="Semaine_Affichage">PlanningProjet!$E$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">PlanningProjet!$A$1:$CN$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">PlanningProjet!$A$1:$CN$35</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="29">
   <si>
     <t>Début du projet :</t>
   </si>
@@ -124,6 +124,12 @@
   <si>
     <t>Ajout des messages + CRUD (service, repository et model)</t>
   </si>
+  <si>
+    <t>Planning effectif :</t>
+  </si>
+  <si>
+    <t>Planning prévu :</t>
+  </si>
 </sst>
 </file>
 
@@ -140,7 +146,7 @@
     <numFmt numFmtId="171" formatCode="d"/>
     <numFmt numFmtId="172" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,6 +343,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1083,6 +1096,13 @@
     <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="171" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="170" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1101,15 +1121,8 @@
     <xf numFmtId="172" fontId="7" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="171" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1168,25 +1181,7 @@
     <cellStyle name="Vérification" xfId="25" builtinId="23" customBuiltin="1"/>
     <cellStyle name="zTexteMasqué" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill>
@@ -1337,15 +1332,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ListeTâches" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="16"/>
-      <tableStyleElement type="headerRow" dxfId="15"/>
-      <tableStyleElement type="totalRow" dxfId="14"/>
-      <tableStyleElement type="firstColumn" dxfId="13"/>
-      <tableStyleElement type="lastColumn" dxfId="12"/>
-      <tableStyleElement type="firstRowStripe" dxfId="11"/>
-      <tableStyleElement type="secondRowStripe" dxfId="10"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="9"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="8"/>
+      <tableStyleElement type="wholeTable" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="totalRow" dxfId="12"/>
+      <tableStyleElement type="firstColumn" dxfId="11"/>
+      <tableStyleElement type="lastColumn" dxfId="10"/>
+      <tableStyleElement type="firstRowStripe" dxfId="9"/>
+      <tableStyleElement type="secondRowStripe" dxfId="8"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="7"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="6"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1707,8 +1702,8 @@
   <dimension ref="A1:CO35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC39" sqref="AC39"/>
+      <pane ySplit="6" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:CN35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1740,158 +1735,161 @@
       <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="72"/>
-      <c r="E2" s="73">
+      <c r="D2" s="75"/>
+      <c r="E2" s="76">
         <v>45609</v>
       </c>
-      <c r="F2" s="73"/>
+      <c r="F2" s="76"/>
       <c r="I2" s="38"/>
     </row>
     <row r="3" spans="1:93" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="73">
+      <c r="D3" s="75"/>
+      <c r="E3" s="76">
         <v>45683</v>
       </c>
-      <c r="F3" s="73"/>
+      <c r="F3" s="76"/>
     </row>
     <row r="4" spans="1:93" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25"/>
-      <c r="C4" s="71" t="s">
+      <c r="B4" s="77" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="72"/>
+      <c r="D4" s="75"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="68">
+      <c r="I4" s="71">
         <f>I5</f>
         <v>45607</v>
       </c>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="69"/>
-      <c r="O4" s="70"/>
-      <c r="P4" s="68">
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="72"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="72"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="71">
         <f>P5</f>
         <v>45614</v>
       </c>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="69"/>
-      <c r="S4" s="69"/>
-      <c r="T4" s="69"/>
-      <c r="U4" s="69"/>
-      <c r="V4" s="70"/>
-      <c r="W4" s="68">
+      <c r="Q4" s="72"/>
+      <c r="R4" s="72"/>
+      <c r="S4" s="72"/>
+      <c r="T4" s="72"/>
+      <c r="U4" s="72"/>
+      <c r="V4" s="73"/>
+      <c r="W4" s="71">
         <f>W5</f>
         <v>45621</v>
       </c>
-      <c r="X4" s="69"/>
-      <c r="Y4" s="69"/>
-      <c r="Z4" s="69"/>
-      <c r="AA4" s="69"/>
-      <c r="AB4" s="69"/>
-      <c r="AC4" s="70"/>
-      <c r="AD4" s="68">
+      <c r="X4" s="72"/>
+      <c r="Y4" s="72"/>
+      <c r="Z4" s="72"/>
+      <c r="AA4" s="72"/>
+      <c r="AB4" s="72"/>
+      <c r="AC4" s="73"/>
+      <c r="AD4" s="71">
         <f t="shared" ref="AD4" si="0">AD5</f>
         <v>45628</v>
       </c>
-      <c r="AE4" s="69"/>
-      <c r="AF4" s="69"/>
-      <c r="AG4" s="69"/>
-      <c r="AH4" s="69"/>
-      <c r="AI4" s="69"/>
-      <c r="AJ4" s="70"/>
-      <c r="AK4" s="68">
+      <c r="AE4" s="72"/>
+      <c r="AF4" s="72"/>
+      <c r="AG4" s="72"/>
+      <c r="AH4" s="72"/>
+      <c r="AI4" s="72"/>
+      <c r="AJ4" s="73"/>
+      <c r="AK4" s="71">
         <f t="shared" ref="AK4" si="1">AK5</f>
         <v>45635</v>
       </c>
-      <c r="AL4" s="69"/>
-      <c r="AM4" s="69"/>
-      <c r="AN4" s="69"/>
-      <c r="AO4" s="69"/>
-      <c r="AP4" s="69"/>
-      <c r="AQ4" s="70"/>
-      <c r="AR4" s="68">
+      <c r="AL4" s="72"/>
+      <c r="AM4" s="72"/>
+      <c r="AN4" s="72"/>
+      <c r="AO4" s="72"/>
+      <c r="AP4" s="72"/>
+      <c r="AQ4" s="73"/>
+      <c r="AR4" s="71">
         <f t="shared" ref="AR4" si="2">AR5</f>
         <v>45642</v>
       </c>
-      <c r="AS4" s="69"/>
-      <c r="AT4" s="69"/>
-      <c r="AU4" s="69"/>
-      <c r="AV4" s="69"/>
-      <c r="AW4" s="69"/>
-      <c r="AX4" s="70"/>
-      <c r="AY4" s="68">
+      <c r="AS4" s="72"/>
+      <c r="AT4" s="72"/>
+      <c r="AU4" s="72"/>
+      <c r="AV4" s="72"/>
+      <c r="AW4" s="72"/>
+      <c r="AX4" s="73"/>
+      <c r="AY4" s="71">
         <f t="shared" ref="AY4" si="3">AY5</f>
         <v>45649</v>
       </c>
-      <c r="AZ4" s="69"/>
-      <c r="BA4" s="69"/>
-      <c r="BB4" s="69"/>
-      <c r="BC4" s="69"/>
-      <c r="BD4" s="69"/>
-      <c r="BE4" s="70"/>
-      <c r="BF4" s="68">
+      <c r="AZ4" s="72"/>
+      <c r="BA4" s="72"/>
+      <c r="BB4" s="72"/>
+      <c r="BC4" s="72"/>
+      <c r="BD4" s="72"/>
+      <c r="BE4" s="73"/>
+      <c r="BF4" s="71">
         <f t="shared" ref="BF4" si="4">BF5</f>
         <v>45656</v>
       </c>
-      <c r="BG4" s="69"/>
-      <c r="BH4" s="69"/>
-      <c r="BI4" s="69"/>
-      <c r="BJ4" s="69"/>
-      <c r="BK4" s="69"/>
-      <c r="BL4" s="70"/>
-      <c r="BM4" s="68">
+      <c r="BG4" s="72"/>
+      <c r="BH4" s="72"/>
+      <c r="BI4" s="72"/>
+      <c r="BJ4" s="72"/>
+      <c r="BK4" s="72"/>
+      <c r="BL4" s="73"/>
+      <c r="BM4" s="71">
         <f t="shared" ref="BM4" si="5">BM5</f>
         <v>45663</v>
       </c>
-      <c r="BN4" s="69"/>
-      <c r="BO4" s="69"/>
-      <c r="BP4" s="69"/>
-      <c r="BQ4" s="69"/>
-      <c r="BR4" s="69"/>
-      <c r="BS4" s="70"/>
-      <c r="BT4" s="68">
+      <c r="BN4" s="72"/>
+      <c r="BO4" s="72"/>
+      <c r="BP4" s="72"/>
+      <c r="BQ4" s="72"/>
+      <c r="BR4" s="72"/>
+      <c r="BS4" s="73"/>
+      <c r="BT4" s="71">
         <f t="shared" ref="BT4" si="6">BT5</f>
         <v>45670</v>
       </c>
-      <c r="BU4" s="69"/>
-      <c r="BV4" s="69"/>
-      <c r="BW4" s="69"/>
-      <c r="BX4" s="69"/>
-      <c r="BY4" s="69"/>
-      <c r="BZ4" s="70"/>
-      <c r="CA4" s="68">
+      <c r="BU4" s="72"/>
+      <c r="BV4" s="72"/>
+      <c r="BW4" s="72"/>
+      <c r="BX4" s="72"/>
+      <c r="BY4" s="72"/>
+      <c r="BZ4" s="73"/>
+      <c r="CA4" s="71">
         <f t="shared" ref="CA4" si="7">CA5</f>
         <v>45677</v>
       </c>
-      <c r="CB4" s="69"/>
-      <c r="CC4" s="69"/>
-      <c r="CD4" s="69"/>
-      <c r="CE4" s="69"/>
-      <c r="CF4" s="69"/>
-      <c r="CG4" s="70"/>
-      <c r="CH4" s="68">
+      <c r="CB4" s="72"/>
+      <c r="CC4" s="72"/>
+      <c r="CD4" s="72"/>
+      <c r="CE4" s="72"/>
+      <c r="CF4" s="72"/>
+      <c r="CG4" s="73"/>
+      <c r="CH4" s="71">
         <f t="shared" ref="CH4" si="8">CH5</f>
         <v>45684</v>
       </c>
-      <c r="CI4" s="69"/>
-      <c r="CJ4" s="69"/>
-      <c r="CK4" s="69"/>
-      <c r="CL4" s="69"/>
-      <c r="CM4" s="69"/>
-      <c r="CN4" s="70"/>
+      <c r="CI4" s="72"/>
+      <c r="CJ4" s="72"/>
+      <c r="CK4" s="72"/>
+      <c r="CL4" s="72"/>
+      <c r="CM4" s="72"/>
+      <c r="CN4" s="73"/>
     </row>
     <row r="5" spans="1:93" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
@@ -2237,7 +2235,7 @@
         <f t="shared" ref="CN5" si="54">CM5+1</f>
         <v>45690</v>
       </c>
-      <c r="CO5" s="77"/>
+      <c r="CO5" s="70"/>
     </row>
     <row r="6" spans="1:93" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25"/>
@@ -3093,7 +3091,7 @@
       <c r="CD11" s="21"/>
       <c r="CE11" s="21"/>
       <c r="CF11" s="22"/>
-      <c r="CG11" s="74"/>
+      <c r="CG11" s="68"/>
       <c r="CH11" s="21"/>
       <c r="CI11" s="21"/>
       <c r="CJ11" s="21"/>
@@ -3510,7 +3508,7 @@
       <c r="CD15" s="21"/>
       <c r="CE15" s="21"/>
       <c r="CF15" s="22"/>
-      <c r="CG15" s="74"/>
+      <c r="CG15" s="68"/>
       <c r="CH15" s="21"/>
       <c r="CI15" s="21"/>
       <c r="CJ15" s="21"/>
@@ -3939,133 +3937,136 @@
     </row>
     <row r="21" spans="1:93" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
-      <c r="C21" s="71" t="s">
+      <c r="B21" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="72"/>
+      <c r="D21" s="75"/>
       <c r="E21" s="7">
         <v>1</v>
       </c>
-      <c r="I21" s="68">
+      <c r="I21" s="71">
         <f>I22</f>
         <v>45607</v>
       </c>
-      <c r="J21" s="69"/>
-      <c r="K21" s="69"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="69"/>
-      <c r="N21" s="69"/>
-      <c r="O21" s="70"/>
-      <c r="P21" s="68">
+      <c r="J21" s="72"/>
+      <c r="K21" s="72"/>
+      <c r="L21" s="72"/>
+      <c r="M21" s="72"/>
+      <c r="N21" s="72"/>
+      <c r="O21" s="73"/>
+      <c r="P21" s="71">
         <f>P22</f>
         <v>45614</v>
       </c>
-      <c r="Q21" s="69"/>
-      <c r="R21" s="69"/>
-      <c r="S21" s="69"/>
-      <c r="T21" s="69"/>
-      <c r="U21" s="69"/>
-      <c r="V21" s="70"/>
-      <c r="W21" s="68">
+      <c r="Q21" s="72"/>
+      <c r="R21" s="72"/>
+      <c r="S21" s="72"/>
+      <c r="T21" s="72"/>
+      <c r="U21" s="72"/>
+      <c r="V21" s="73"/>
+      <c r="W21" s="71">
         <f>W22</f>
         <v>45621</v>
       </c>
-      <c r="X21" s="69"/>
-      <c r="Y21" s="69"/>
-      <c r="Z21" s="69"/>
-      <c r="AA21" s="69"/>
-      <c r="AB21" s="69"/>
-      <c r="AC21" s="70"/>
-      <c r="AD21" s="68">
+      <c r="X21" s="72"/>
+      <c r="Y21" s="72"/>
+      <c r="Z21" s="72"/>
+      <c r="AA21" s="72"/>
+      <c r="AB21" s="72"/>
+      <c r="AC21" s="73"/>
+      <c r="AD21" s="71">
         <f t="shared" ref="AD21" si="59">AD22</f>
         <v>45628</v>
       </c>
-      <c r="AE21" s="69"/>
-      <c r="AF21" s="69"/>
-      <c r="AG21" s="69"/>
-      <c r="AH21" s="69"/>
-      <c r="AI21" s="69"/>
-      <c r="AJ21" s="70"/>
-      <c r="AK21" s="68">
+      <c r="AE21" s="72"/>
+      <c r="AF21" s="72"/>
+      <c r="AG21" s="72"/>
+      <c r="AH21" s="72"/>
+      <c r="AI21" s="72"/>
+      <c r="AJ21" s="73"/>
+      <c r="AK21" s="71">
         <f t="shared" ref="AK21" si="60">AK22</f>
         <v>45635</v>
       </c>
-      <c r="AL21" s="69"/>
-      <c r="AM21" s="69"/>
-      <c r="AN21" s="69"/>
-      <c r="AO21" s="69"/>
-      <c r="AP21" s="69"/>
-      <c r="AQ21" s="70"/>
-      <c r="AR21" s="68">
+      <c r="AL21" s="72"/>
+      <c r="AM21" s="72"/>
+      <c r="AN21" s="72"/>
+      <c r="AO21" s="72"/>
+      <c r="AP21" s="72"/>
+      <c r="AQ21" s="73"/>
+      <c r="AR21" s="71">
         <f t="shared" ref="AR21" si="61">AR22</f>
         <v>45642</v>
       </c>
-      <c r="AS21" s="69"/>
-      <c r="AT21" s="69"/>
-      <c r="AU21" s="69"/>
-      <c r="AV21" s="69"/>
-      <c r="AW21" s="69"/>
-      <c r="AX21" s="70"/>
-      <c r="AY21" s="68">
+      <c r="AS21" s="72"/>
+      <c r="AT21" s="72"/>
+      <c r="AU21" s="72"/>
+      <c r="AV21" s="72"/>
+      <c r="AW21" s="72"/>
+      <c r="AX21" s="73"/>
+      <c r="AY21" s="71">
         <f t="shared" ref="AY21" si="62">AY22</f>
         <v>45649</v>
       </c>
-      <c r="AZ21" s="69"/>
-      <c r="BA21" s="69"/>
-      <c r="BB21" s="69"/>
-      <c r="BC21" s="69"/>
-      <c r="BD21" s="69"/>
-      <c r="BE21" s="70"/>
-      <c r="BF21" s="68">
+      <c r="AZ21" s="72"/>
+      <c r="BA21" s="72"/>
+      <c r="BB21" s="72"/>
+      <c r="BC21" s="72"/>
+      <c r="BD21" s="72"/>
+      <c r="BE21" s="73"/>
+      <c r="BF21" s="71">
         <f t="shared" ref="BF21" si="63">BF22</f>
         <v>45656</v>
       </c>
-      <c r="BG21" s="69"/>
-      <c r="BH21" s="69"/>
-      <c r="BI21" s="69"/>
-      <c r="BJ21" s="69"/>
-      <c r="BK21" s="69"/>
-      <c r="BL21" s="70"/>
-      <c r="BM21" s="68">
+      <c r="BG21" s="72"/>
+      <c r="BH21" s="72"/>
+      <c r="BI21" s="72"/>
+      <c r="BJ21" s="72"/>
+      <c r="BK21" s="72"/>
+      <c r="BL21" s="73"/>
+      <c r="BM21" s="71">
         <f t="shared" ref="BM21" si="64">BM22</f>
         <v>45663</v>
       </c>
-      <c r="BN21" s="69"/>
-      <c r="BO21" s="69"/>
-      <c r="BP21" s="69"/>
-      <c r="BQ21" s="69"/>
-      <c r="BR21" s="69"/>
-      <c r="BS21" s="70"/>
-      <c r="BT21" s="68">
+      <c r="BN21" s="72"/>
+      <c r="BO21" s="72"/>
+      <c r="BP21" s="72"/>
+      <c r="BQ21" s="72"/>
+      <c r="BR21" s="72"/>
+      <c r="BS21" s="73"/>
+      <c r="BT21" s="71">
         <f t="shared" ref="BT21" si="65">BT22</f>
         <v>45670</v>
       </c>
-      <c r="BU21" s="69"/>
-      <c r="BV21" s="69"/>
-      <c r="BW21" s="69"/>
-      <c r="BX21" s="69"/>
-      <c r="BY21" s="69"/>
-      <c r="BZ21" s="70"/>
-      <c r="CA21" s="68">
+      <c r="BU21" s="72"/>
+      <c r="BV21" s="72"/>
+      <c r="BW21" s="72"/>
+      <c r="BX21" s="72"/>
+      <c r="BY21" s="72"/>
+      <c r="BZ21" s="73"/>
+      <c r="CA21" s="71">
         <f t="shared" ref="CA21" si="66">CA22</f>
         <v>45677</v>
       </c>
-      <c r="CB21" s="69"/>
-      <c r="CC21" s="69"/>
-      <c r="CD21" s="69"/>
-      <c r="CE21" s="69"/>
-      <c r="CF21" s="69"/>
-      <c r="CG21" s="70"/>
-      <c r="CH21" s="68">
+      <c r="CB21" s="72"/>
+      <c r="CC21" s="72"/>
+      <c r="CD21" s="72"/>
+      <c r="CE21" s="72"/>
+      <c r="CF21" s="72"/>
+      <c r="CG21" s="73"/>
+      <c r="CH21" s="71">
         <f t="shared" ref="CH21" si="67">CH22</f>
         <v>45684</v>
       </c>
-      <c r="CI21" s="69"/>
-      <c r="CJ21" s="69"/>
-      <c r="CK21" s="69"/>
-      <c r="CL21" s="69"/>
-      <c r="CM21" s="69"/>
-      <c r="CN21" s="70"/>
+      <c r="CI21" s="72"/>
+      <c r="CJ21" s="72"/>
+      <c r="CK21" s="72"/>
+      <c r="CL21" s="72"/>
+      <c r="CM21" s="72"/>
+      <c r="CN21" s="73"/>
     </row>
     <row r="22" spans="1:93" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25"/>
@@ -4335,7 +4336,7 @@
         <f t="shared" ref="BU22" si="126">BT22+1</f>
         <v>45671</v>
       </c>
-      <c r="BV22" s="75">
+      <c r="BV22" s="49">
         <f>BU22+1</f>
         <v>45672</v>
       </c>
@@ -4359,11 +4360,11 @@
         <f t="shared" ref="CA22" si="130">BZ22+1</f>
         <v>45677</v>
       </c>
-      <c r="CB22" s="75">
+      <c r="CB22" s="49">
         <f t="shared" ref="CB22" si="131">CA22+1</f>
         <v>45678</v>
       </c>
-      <c r="CC22" s="75">
+      <c r="CC22" s="49">
         <f>CB22+1</f>
         <v>45679</v>
       </c>
@@ -4387,11 +4388,11 @@
         <f t="shared" ref="CH22" si="135">CG22+1</f>
         <v>45684</v>
       </c>
-      <c r="CI22" s="75">
+      <c r="CI22" s="49">
         <f t="shared" ref="CI22" si="136">CH22+1</f>
         <v>45685</v>
       </c>
-      <c r="CJ22" s="75">
+      <c r="CJ22" s="49">
         <f t="shared" ref="CJ22" si="137">CI22+1</f>
         <v>45686</v>
       </c>
@@ -4411,7 +4412,7 @@
         <f t="shared" ref="CN22" si="141">CM22+1</f>
         <v>45690</v>
       </c>
-      <c r="CO22" s="76"/>
+      <c r="CO22" s="69"/>
     </row>
     <row r="23" spans="1:93" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="25"/>
@@ -5171,7 +5172,7 @@
       <c r="CD27" s="21"/>
       <c r="CE27" s="21"/>
       <c r="CF27" s="22"/>
-      <c r="CG27" s="74"/>
+      <c r="CG27" s="68"/>
       <c r="CH27" s="21"/>
       <c r="CI27" s="21"/>
       <c r="CJ27" s="21"/>
@@ -5685,7 +5686,7 @@
       <c r="CD32" s="21"/>
       <c r="CE32" s="21"/>
       <c r="CF32" s="22"/>
-      <c r="CG32" s="74"/>
+      <c r="CG32" s="68"/>
       <c r="CH32" s="21"/>
       <c r="CI32" s="21"/>
       <c r="CJ32" s="21"/>
@@ -6009,6 +6010,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="BM21:BS21"/>
+    <mergeCell ref="BT21:BZ21"/>
+    <mergeCell ref="CA21:CG21"/>
+    <mergeCell ref="CH21:CN21"/>
+    <mergeCell ref="AD21:AJ21"/>
+    <mergeCell ref="AK21:AQ21"/>
+    <mergeCell ref="AR21:AX21"/>
+    <mergeCell ref="AY21:BE21"/>
+    <mergeCell ref="BF21:BL21"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="I21:O21"/>
+    <mergeCell ref="P21:V21"/>
+    <mergeCell ref="W21:AC21"/>
     <mergeCell ref="BM4:BS4"/>
     <mergeCell ref="BT4:BZ4"/>
     <mergeCell ref="CA4:CG4"/>
@@ -6025,22 +6040,64 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="I21:O21"/>
-    <mergeCell ref="P21:V21"/>
-    <mergeCell ref="W21:AC21"/>
-    <mergeCell ref="AD21:AJ21"/>
-    <mergeCell ref="AK21:AQ21"/>
-    <mergeCell ref="AR21:AX21"/>
-    <mergeCell ref="AY21:BE21"/>
-    <mergeCell ref="BF21:BL21"/>
-    <mergeCell ref="BM21:BS21"/>
-    <mergeCell ref="BT21:BZ21"/>
-    <mergeCell ref="CA21:CG21"/>
-    <mergeCell ref="CH21:CN21"/>
   </mergeCells>
   <phoneticPr fontId="27" type="noConversion"/>
+  <conditionalFormatting sqref="C17:C18">
+    <cfRule type="dataBar" priority="14">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{6557F7AA-4413-4C5B-897B-DA48C7591888}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33:C34">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{ABA16467-6632-44BB-856B-431AF1650BBB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:D8 D7">
+    <cfRule type="dataBar" priority="58">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B0389232-4C98-4A03-AD0E-39F63BAD1F53}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24:D24">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F415D66B-155F-401F-B13B-FD8672886708}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D9:D19">
     <cfRule type="dataBar" priority="13">
       <dataBar>
@@ -6055,8 +6112,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17:C18">
-    <cfRule type="dataBar" priority="14">
+  <conditionalFormatting sqref="D25:D35">
+    <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -6064,21 +6121,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6557F7AA-4413-4C5B-897B-DA48C7591888}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8:D8 D7">
-    <cfRule type="dataBar" priority="58">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0" tint="-0.249977111117893"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B0389232-4C98-4A03-AD0E-39F63BAD1F53}</x14:id>
+          <x14:id>{378BE8B3-6310-47A9-A94C-4BE65588BEE0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -6111,14 +6154,6 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8:AB9 AD8:AW9 AY8:BR9 BT8:CM9 I10:R10 T10:AB10 AD10:AM10 AO10:AW10 AY10:BH10 BJ10:BR10 BT10:CC10 CE10:CM10 AC8:AC15 AX8:AX15 BS8:BS15 I11:AB15 AD11:AW15 AY11:BR15 BT11:CM15 I7:CM7 I16:CM19">
-    <cfRule type="expression" dxfId="7" priority="71">
-      <formula>AND(début_tâche&lt;=I$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="72" stopIfTrue="1">
-      <formula>AND(fin_tâche&gt;=I$5,début_tâche&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I24:AB25 AD24:AW25 AY24:BR25 BT24:CM25 AC24:AC35 AX24:AX35 BS24:BS35 I26:R26 T26:AB26 AD26:AM26 AO26:AW26 AY26:BH26 BJ26:BR26 BT26:CC26 CE26:CM26 I27:AB35 AD27:AW35 AY27:BR35 BT27:CM35">
     <cfRule type="expression" dxfId="5" priority="8">
       <formula>AND(début_tâche&lt;=I$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$5)</formula>
@@ -6127,54 +6162,20 @@
       <formula>AND(fin_tâche&gt;=I$5,début_tâche&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I7:CM7 I8:AB9 AD8:AW9 AY8:BR9 BT8:CM9 AC8:AC15 AX8:AX15 BS8:BS15 I10:R10 T10:AB10 AD10:AM10 AO10:AW10 AY10:BH10 BJ10:BR10 BT10:CC10 CE10:CM10 I11:AB15 AD11:AW15 AY11:BR15 BT11:CM15 I16:CM19">
+    <cfRule type="expression" dxfId="3" priority="71">
+      <formula>AND(début_tâche&lt;=I$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="72" stopIfTrue="1">
+      <formula>AND(fin_tâche&gt;=I$5,début_tâche&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="CN7:CN19 CN24:CN35">
-    <cfRule type="expression" dxfId="3" priority="75">
+    <cfRule type="expression" dxfId="1" priority="75">
       <formula>AND(début_tâche&lt;=CN$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=CN$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="76" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=CN$5,début_tâche&lt;#REF!)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25:D35">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0" tint="-0.249977111117893"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{378BE8B3-6310-47A9-A94C-4BE65588BEE0}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C33:C34">
-    <cfRule type="dataBar" priority="2">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0" tint="-0.249977111117893"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{ABA16467-6632-44BB-856B-431AF1650BBB}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24:D24">
-    <cfRule type="dataBar" priority="3">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0" tint="-0.249977111117893"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{F415D66B-155F-401F-B13B-FD8672886708}</x14:id>
-        </ext>
-      </extLst>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -6184,7 +6185,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="30" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="41" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -6194,6 +6195,66 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6557F7AA-4413-4C5B-897B-DA48C7591888}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C17:C18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{ABA16467-6632-44BB-856B-431AF1650BBB}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C33:C34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B0389232-4C98-4A03-AD0E-39F63BAD1F53}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C8:D8 D7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F415D66B-155F-401F-B13B-FD8672886708}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C24:D24</xm:sqref>
+        </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{8D9C14ED-16EA-4407-989D-898CDC2472E9}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
@@ -6210,7 +6271,7 @@
           <xm:sqref>D9:D19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6557F7AA-4413-4C5B-897B-DA48C7591888}">
+          <x14:cfRule type="dataBar" id="{378BE8B3-6310-47A9-A94C-4BE65588BEE0}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -6222,22 +6283,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C17:C18</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B0389232-4C98-4A03-AD0E-39F63BAD1F53}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>C8:D8 D7</xm:sqref>
+          <xm:sqref>D25:D35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{D5A7D14F-9061-43B3-9219-F1FD206AE2FB}">
@@ -6268,51 +6314,6 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>G24</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{378BE8B3-6310-47A9-A94C-4BE65588BEE0}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D25:D35</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{ABA16467-6632-44BB-856B-431AF1650BBB}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>C33:C34</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F415D66B-155F-401F-B13B-FD8672886708}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>C24:D24</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -6609,15 +6610,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -6635,6 +6627,15 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6659,28 +6660,28 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>